<commit_message>
Analisi fase 1 fatta
</commit_message>
<xml_diff>
--- a/Analisi approfondita sovrapponibili.xlsx
+++ b/Analisi approfondita sovrapponibili.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documenti\repositories\Super Mario Deep Maker 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604F285E-2D06-4FAB-9D09-A60C24C6FBDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599F3DFF-8C44-4EE7-ADA3-E377629A17CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="157">
   <si>
     <t>Nome</t>
   </si>
@@ -470,20 +470,44 @@
     <t>Freccia</t>
   </si>
   <si>
-    <t>Background no se stesso</t>
-  </si>
-  <si>
     <t>10 coin</t>
   </si>
   <si>
     <t>Snake</t>
+  </si>
+  <si>
+    <t>CheckPoint Flag</t>
+  </si>
+  <si>
+    <t>Pink coin</t>
+  </si>
+  <si>
+    <t>Segomma</t>
+  </si>
+  <si>
+    <t>Lift</t>
+  </si>
+  <si>
+    <t>Background 2</t>
+  </si>
+  <si>
+    <t>Background 3</t>
+  </si>
+  <si>
+    <t>Background 4</t>
+  </si>
+  <si>
+    <t>Background 5</t>
+  </si>
+  <si>
+    <t>Background 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,8 +515,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,6 +540,72 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDA9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCF20E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9ADAD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB9FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,16 +622,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB9FFFF"/>
+      <color rgb="FFF9ADAD"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFCCF20E"/>
+      <color rgb="FFFDA9F9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -802,11 +927,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q121"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:S121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,11 +944,10 @@
     <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -857,19 +982,25 @@
         <v>145</v>
       </c>
       <c r="N1" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="O1" t="s">
-        <v>101</v>
+        <v>147</v>
       </c>
       <c r="P1" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="Q1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="R1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -883,7 +1014,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -897,7 +1028,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -911,7 +1042,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -925,7 +1056,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -954,7 +1085,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -968,7 +1099,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -982,7 +1113,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -996,7 +1127,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1025,7 +1156,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1060,7 +1191,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1074,7 +1205,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1085,10 +1216,10 @@
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1102,7 +1233,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1116,7 +1247,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1130,7 +1261,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1144,7 +1275,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1158,7 +1289,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1190,7 +1321,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1204,7 +1335,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1218,7 +1349,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1232,7 +1363,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1246,7 +1377,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1260,7 +1391,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1274,7 +1405,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1288,7 +1419,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1302,7 +1433,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1337,7 +1468,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1372,7 +1503,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1386,7 +1517,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1400,7 +1531,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1414,7 +1545,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1428,7 +1559,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1442,7 +1573,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1456,7 +1587,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -1470,7 +1601,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -1484,7 +1615,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1495,13 +1626,13 @@
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E38" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1539,7 +1670,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -1577,7 +1708,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1591,7 +1722,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1605,7 +1736,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1619,7 +1750,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1633,7 +1764,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1647,7 +1778,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -1661,7 +1792,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -1675,7 +1806,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1689,7 +1820,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -1703,7 +1834,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -1717,7 +1848,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -1731,7 +1862,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1745,7 +1876,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1759,7 +1890,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1773,7 +1904,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -1787,7 +1918,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -1801,7 +1932,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -1811,6 +1942,9 @@
       <c r="C57" t="s">
         <v>65</v>
       </c>
+      <c r="D57" t="s">
+        <v>142</v>
+      </c>
       <c r="E57" t="s">
         <v>134</v>
       </c>
@@ -1839,7 +1973,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1853,7 +1987,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1867,7 +2001,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1881,7 +2015,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -1891,8 +2025,11 @@
       <c r="C61" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -1906,7 +2043,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -1920,7 +2057,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1934,7 +2071,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -1948,7 +2085,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -1959,10 +2096,10 @@
         <v>76</v>
       </c>
       <c r="D66" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1976,7 +2113,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -1990,7 +2127,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -2004,7 +2141,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -2015,7 +2152,7 @@
         <v>80</v>
       </c>
       <c r="D70" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E70" t="s">
         <v>134</v>
@@ -2044,11 +2181,8 @@
       <c r="M70" t="s">
         <v>134</v>
       </c>
-      <c r="N70" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>33</v>
       </c>
@@ -2062,7 +2196,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -2076,7 +2210,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -2090,7 +2224,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -2104,7 +2238,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>33</v>
       </c>
@@ -2118,7 +2252,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -2132,7 +2266,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>33</v>
       </c>
@@ -2146,7 +2280,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -2160,7 +2294,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -2174,7 +2308,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -2188,7 +2322,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -2202,7 +2336,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -2216,7 +2350,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>33</v>
       </c>
@@ -2230,7 +2364,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -2241,10 +2375,10 @@
         <v>93</v>
       </c>
       <c r="D84" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -2255,10 +2389,10 @@
         <v>94</v>
       </c>
       <c r="D85" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -2269,10 +2403,10 @@
         <v>95</v>
       </c>
       <c r="D86" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -2286,7 +2420,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -2300,7 +2434,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -2310,6 +2444,9 @@
       <c r="C89" t="s">
         <v>98</v>
       </c>
+      <c r="D89" t="s">
+        <v>135</v>
+      </c>
       <c r="E89" t="s">
         <v>134</v>
       </c>
@@ -2338,16 +2475,13 @@
         <v>134</v>
       </c>
       <c r="N89" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O89" t="s">
         <v>133</v>
       </c>
-      <c r="P89" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -2357,8 +2491,11 @@
       <c r="C90" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>33</v>
       </c>
@@ -2368,8 +2505,11 @@
       <c r="C91" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -2410,13 +2550,10 @@
         <v>134</v>
       </c>
       <c r="N92" t="s">
-        <v>134</v>
-      </c>
-      <c r="O92" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -2426,8 +2563,11 @@
       <c r="C93" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -2437,8 +2577,41 @@
       <c r="C94" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>103</v>
+      </c>
+      <c r="E94" t="s">
+        <v>133</v>
+      </c>
+      <c r="F94" t="s">
+        <v>134</v>
+      </c>
+      <c r="G94" t="s">
+        <v>134</v>
+      </c>
+      <c r="H94" t="s">
+        <v>133</v>
+      </c>
+      <c r="I94" t="s">
+        <v>133</v>
+      </c>
+      <c r="J94" t="s">
+        <v>133</v>
+      </c>
+      <c r="K94" t="s">
+        <v>133</v>
+      </c>
+      <c r="L94" t="s">
+        <v>134</v>
+      </c>
+      <c r="N94" t="s">
+        <v>133</v>
+      </c>
+      <c r="O94" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -2452,7 +2625,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -2462,8 +2635,11 @@
       <c r="C96" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -2473,8 +2649,17 @@
       <c r="C97" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>130</v>
+      </c>
+      <c r="E97" t="s">
+        <v>133</v>
+      </c>
+      <c r="F97" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>3</v>
       </c>
@@ -2488,7 +2673,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -2498,8 +2683,11 @@
       <c r="C99" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>3</v>
       </c>
@@ -2513,7 +2701,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -2527,7 +2715,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -2537,8 +2725,11 @@
       <c r="C102" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>33</v>
       </c>
@@ -2548,8 +2739,11 @@
       <c r="C103" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>3</v>
       </c>
@@ -2563,7 +2757,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>3</v>
       </c>
@@ -2577,7 +2771,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -2591,7 +2785,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -2601,8 +2795,11 @@
       <c r="C107" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -2616,7 +2813,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>3</v>
       </c>
@@ -2630,7 +2827,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -2644,7 +2841,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>33</v>
       </c>
@@ -2658,7 +2855,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -2672,7 +2869,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>33</v>
       </c>
@@ -2686,7 +2883,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>16</v>
       </c>
@@ -2700,7 +2897,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>16</v>
       </c>
@@ -2714,7 +2911,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>3</v>
       </c>
@@ -2728,7 +2925,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -2742,7 +2939,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -2756,7 +2953,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>3</v>
       </c>
@@ -2770,7 +2967,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>16</v>
       </c>
@@ -2784,7 +2981,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>119</v>
       </c>
@@ -2796,7 +2993,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L121" xr:uid="{AF469F71-5011-4551-9995-E4BE0EFC6196}"/>
+  <autoFilter ref="A1:L121" xr:uid="{AF469F71-5011-4551-9995-E4BE0EFC6196}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Background no se stesso"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4130,661 +4333,1247 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76425061-D43B-44F5-ADB3-D0ABE7860380}">
-  <dimension ref="D8:Q22"/>
+  <dimension ref="B8:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>136</v>
       </c>
-      <c r="E8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="G8" t="s">
+      <c r="E8" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H8" t="s">
+      <c r="F8" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="I8" t="s">
+      <c r="G8" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="J8" t="s">
+      <c r="H8" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="K8" t="s">
+      <c r="I8" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="L8" t="s">
+      <c r="J8" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="M8" t="s">
+      <c r="K8" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="N8" t="s">
+      <c r="L8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="O8" t="s">
+      <c r="N8" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="T8" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" t="s">
+        <v>134</v>
+      </c>
+      <c r="G9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I9" t="s">
+        <v>134</v>
+      </c>
+      <c r="J9" t="s">
+        <v>134</v>
+      </c>
+      <c r="K9" t="s">
+        <v>134</v>
+      </c>
+      <c r="L9" t="s">
+        <v>134</v>
+      </c>
+      <c r="M9" t="s">
+        <v>134</v>
+      </c>
+      <c r="N9" t="s">
+        <v>133</v>
+      </c>
+      <c r="O9" t="s">
+        <v>133</v>
+      </c>
+      <c r="P9" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>134</v>
+      </c>
+      <c r="R9" t="s">
+        <v>134</v>
+      </c>
+      <c r="S9" t="s">
+        <v>134</v>
+      </c>
+      <c r="T9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G10" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" t="s">
+        <v>134</v>
+      </c>
+      <c r="I10" t="s">
+        <v>134</v>
+      </c>
+      <c r="J10" t="s">
+        <v>134</v>
+      </c>
+      <c r="K10" t="s">
+        <v>133</v>
+      </c>
+      <c r="L10" t="s">
+        <v>134</v>
+      </c>
+      <c r="M10" t="s">
+        <v>134</v>
+      </c>
+      <c r="N10" t="s">
+        <v>134</v>
+      </c>
+      <c r="O10" t="s">
+        <v>134</v>
+      </c>
+      <c r="P10" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>134</v>
+      </c>
+      <c r="R10" t="s">
+        <v>134</v>
+      </c>
+      <c r="S10" t="s">
+        <v>134</v>
+      </c>
+      <c r="T10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" t="s">
+        <v>133</v>
+      </c>
+      <c r="G11" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" t="s">
+        <v>133</v>
+      </c>
+      <c r="J11" t="s">
+        <v>133</v>
+      </c>
+      <c r="K11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L11" t="s">
+        <v>134</v>
+      </c>
+      <c r="M11" t="s">
+        <v>133</v>
+      </c>
+      <c r="N11" t="s">
+        <v>133</v>
+      </c>
+      <c r="O11" t="s">
+        <v>133</v>
+      </c>
+      <c r="P11" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>134</v>
+      </c>
+      <c r="R11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S11" t="s">
+        <v>134</v>
+      </c>
+      <c r="T11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H12" t="s">
+        <v>133</v>
+      </c>
+      <c r="I12" t="s">
+        <v>133</v>
+      </c>
+      <c r="J12" t="s">
+        <v>133</v>
+      </c>
+      <c r="K12" t="s">
+        <v>134</v>
+      </c>
+      <c r="L12" t="s">
+        <v>134</v>
+      </c>
+      <c r="M12" t="s">
+        <v>133</v>
+      </c>
+      <c r="N12" t="s">
+        <v>133</v>
+      </c>
+      <c r="O12" t="s">
+        <v>133</v>
+      </c>
+      <c r="P12" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>134</v>
+      </c>
+      <c r="R12" t="s">
+        <v>134</v>
+      </c>
+      <c r="S12" t="s">
+        <v>134</v>
+      </c>
+      <c r="T12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I13" t="s">
+        <v>134</v>
+      </c>
+      <c r="J13" t="s">
+        <v>134</v>
+      </c>
+      <c r="K13" t="s">
+        <v>134</v>
+      </c>
+      <c r="L13" t="s">
+        <v>134</v>
+      </c>
+      <c r="M13" t="s">
+        <v>134</v>
+      </c>
+      <c r="N13" t="s">
+        <v>134</v>
+      </c>
+      <c r="O13" t="s">
+        <v>134</v>
+      </c>
+      <c r="P13" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>134</v>
+      </c>
+      <c r="R13" t="s">
+        <v>134</v>
+      </c>
+      <c r="S13" t="s">
+        <v>134</v>
+      </c>
+      <c r="T13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I14" t="s">
+        <v>134</v>
+      </c>
+      <c r="J14" t="s">
+        <v>133</v>
+      </c>
+      <c r="K14" t="s">
+        <v>133</v>
+      </c>
+      <c r="L14" t="s">
+        <v>134</v>
+      </c>
+      <c r="M14" t="s">
+        <v>133</v>
+      </c>
+      <c r="N14" t="s">
+        <v>133</v>
+      </c>
+      <c r="O14" t="s">
+        <v>134</v>
+      </c>
+      <c r="P14" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>134</v>
+      </c>
+      <c r="R14" t="s">
+        <v>134</v>
+      </c>
+      <c r="S14" t="s">
+        <v>134</v>
+      </c>
+      <c r="T14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J15" t="s">
+        <v>134</v>
+      </c>
+      <c r="K15" t="s">
+        <v>134</v>
+      </c>
+      <c r="L15" t="s">
+        <v>134</v>
+      </c>
+      <c r="M15" t="s">
+        <v>133</v>
+      </c>
+      <c r="N15" t="s">
+        <v>133</v>
+      </c>
+      <c r="O15" t="s">
+        <v>133</v>
+      </c>
+      <c r="P15" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>134</v>
+      </c>
+      <c r="R15" t="s">
+        <v>134</v>
+      </c>
+      <c r="S15" t="s">
+        <v>134</v>
+      </c>
+      <c r="T15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" t="s">
+        <v>134</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K16" t="s">
+        <v>134</v>
+      </c>
+      <c r="L16" t="s">
+        <v>134</v>
+      </c>
+      <c r="M16" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16" t="s">
+        <v>133</v>
+      </c>
+      <c r="O16" t="s">
+        <v>133</v>
+      </c>
+      <c r="P16" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>134</v>
+      </c>
+      <c r="R16" t="s">
+        <v>134</v>
+      </c>
+      <c r="S16" t="s">
+        <v>134</v>
+      </c>
+      <c r="T16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" t="s">
+        <v>133</v>
+      </c>
+      <c r="I17" t="s">
+        <v>134</v>
+      </c>
+      <c r="J17" t="s">
+        <v>134</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="L17" t="s">
+        <v>134</v>
+      </c>
+      <c r="M17" t="s">
+        <v>134</v>
+      </c>
+      <c r="N17" t="s">
+        <v>133</v>
+      </c>
+      <c r="O17" t="s">
+        <v>134</v>
+      </c>
+      <c r="P17" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>134</v>
+      </c>
+      <c r="R17" t="s">
+        <v>134</v>
+      </c>
+      <c r="S17" t="s">
+        <v>134</v>
+      </c>
+      <c r="T17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" t="s">
+        <v>134</v>
+      </c>
+      <c r="G18" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" t="s">
+        <v>134</v>
+      </c>
+      <c r="I18" t="s">
+        <v>134</v>
+      </c>
+      <c r="J18" t="s">
+        <v>134</v>
+      </c>
+      <c r="K18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N18" t="s">
+        <v>134</v>
+      </c>
+      <c r="O18" t="s">
+        <v>134</v>
+      </c>
+      <c r="P18" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>134</v>
+      </c>
+      <c r="R18" t="s">
+        <v>134</v>
+      </c>
+      <c r="S18" t="s">
+        <v>134</v>
+      </c>
+      <c r="T18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="N19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O19" t="s">
+        <v>133</v>
+      </c>
+      <c r="P19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="C20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I20" t="s">
+        <v>133</v>
+      </c>
+      <c r="J20" t="s">
+        <v>133</v>
+      </c>
+      <c r="K20" t="s">
+        <v>134</v>
+      </c>
+      <c r="L20" t="s">
+        <v>134</v>
+      </c>
+      <c r="M20" t="s">
+        <v>133</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="O20" t="s">
+        <v>133</v>
+      </c>
+      <c r="P20" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>134</v>
+      </c>
+      <c r="R20" t="s">
+        <v>134</v>
+      </c>
+      <c r="S20" t="s">
+        <v>134</v>
+      </c>
+      <c r="T20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J21" t="s">
+        <v>133</v>
+      </c>
+      <c r="K21" t="s">
+        <v>134</v>
+      </c>
+      <c r="L21" t="s">
+        <v>134</v>
+      </c>
+      <c r="M21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="P21" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>134</v>
+      </c>
+      <c r="R21" t="s">
+        <v>134</v>
+      </c>
+      <c r="S21" t="s">
+        <v>134</v>
+      </c>
+      <c r="T21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" t="s">
+        <v>133</v>
+      </c>
+      <c r="I22" t="s">
+        <v>133</v>
+      </c>
+      <c r="J22" t="s">
+        <v>134</v>
+      </c>
+      <c r="K22" t="s">
+        <v>134</v>
+      </c>
+      <c r="L22" t="s">
+        <v>134</v>
+      </c>
+      <c r="M22" t="s">
+        <v>133</v>
+      </c>
+      <c r="N22" t="s">
+        <v>133</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>134</v>
+      </c>
+      <c r="R22" t="s">
+        <v>134</v>
+      </c>
+      <c r="S22" t="s">
+        <v>134</v>
+      </c>
+      <c r="T22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" t="s">
+        <v>134</v>
+      </c>
+      <c r="G23" t="s">
+        <v>134</v>
+      </c>
+      <c r="H23" t="s">
+        <v>134</v>
+      </c>
+      <c r="I23" t="s">
+        <v>134</v>
+      </c>
+      <c r="J23" t="s">
+        <v>134</v>
+      </c>
+      <c r="K23" t="s">
+        <v>134</v>
+      </c>
+      <c r="L23" t="s">
+        <v>134</v>
+      </c>
+      <c r="M23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N23" t="s">
+        <v>134</v>
+      </c>
+      <c r="O23" t="s">
+        <v>134</v>
+      </c>
+      <c r="P23" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="R23" t="s">
+        <v>134</v>
+      </c>
+      <c r="S23" t="s">
+        <v>134</v>
+      </c>
+      <c r="T23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" t="s">
+        <v>134</v>
+      </c>
+      <c r="H24" t="s">
+        <v>134</v>
+      </c>
+      <c r="I24" t="s">
+        <v>134</v>
+      </c>
+      <c r="J24" t="s">
+        <v>134</v>
+      </c>
+      <c r="K24" t="s">
+        <v>134</v>
+      </c>
+      <c r="L24" t="s">
+        <v>134</v>
+      </c>
+      <c r="M24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N24" t="s">
+        <v>134</v>
+      </c>
+      <c r="O24" t="s">
+        <v>134</v>
+      </c>
+      <c r="P24" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>134</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="S24" t="s">
+        <v>134</v>
+      </c>
+      <c r="T24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" t="s">
+        <v>134</v>
+      </c>
+      <c r="H25" t="s">
+        <v>134</v>
+      </c>
+      <c r="I25" t="s">
+        <v>134</v>
+      </c>
+      <c r="J25" t="s">
+        <v>134</v>
+      </c>
+      <c r="K25" t="s">
+        <v>134</v>
+      </c>
+      <c r="L25" t="s">
+        <v>134</v>
+      </c>
+      <c r="M25" t="s">
+        <v>134</v>
+      </c>
+      <c r="N25" t="s">
+        <v>134</v>
+      </c>
+      <c r="O25" t="s">
+        <v>134</v>
+      </c>
+      <c r="P25" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>134</v>
+      </c>
+      <c r="R25" t="s">
+        <v>134</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="T25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G26" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" t="s">
+        <v>134</v>
+      </c>
+      <c r="I26" t="s">
+        <v>134</v>
+      </c>
+      <c r="J26" t="s">
+        <v>134</v>
+      </c>
+      <c r="K26" t="s">
+        <v>134</v>
+      </c>
+      <c r="L26" t="s">
+        <v>134</v>
+      </c>
+      <c r="M26" t="s">
+        <v>134</v>
+      </c>
+      <c r="N26" t="s">
+        <v>134</v>
+      </c>
+      <c r="O26" t="s">
+        <v>134</v>
+      </c>
+      <c r="P26" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>134</v>
+      </c>
+      <c r="R26" t="s">
+        <v>134</v>
+      </c>
+      <c r="S26" t="s">
+        <v>134</v>
+      </c>
+      <c r="T26" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F9" t="s">
-        <v>134</v>
-      </c>
-      <c r="G9" t="s">
-        <v>134</v>
-      </c>
-      <c r="H9" t="s">
-        <v>134</v>
-      </c>
-      <c r="I9" t="s">
-        <v>134</v>
-      </c>
-      <c r="J9" t="s">
-        <v>134</v>
-      </c>
-      <c r="K9" t="s">
-        <v>134</v>
-      </c>
-      <c r="L9" t="s">
-        <v>134</v>
-      </c>
-      <c r="M9" t="s">
-        <v>134</v>
-      </c>
-      <c r="N9" t="s">
-        <v>134</v>
-      </c>
-      <c r="O9" t="s">
-        <v>134</v>
-      </c>
-      <c r="P9" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" t="s">
-        <v>137</v>
-      </c>
-      <c r="G10" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" t="s">
-        <v>134</v>
-      </c>
-      <c r="I10" t="s">
-        <v>134</v>
-      </c>
-      <c r="J10" t="s">
-        <v>134</v>
-      </c>
-      <c r="M10" t="s">
-        <v>133</v>
-      </c>
-      <c r="N10" t="s">
-        <v>134</v>
-      </c>
-      <c r="O10" t="s">
-        <v>134</v>
-      </c>
-      <c r="P10" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F11" t="s">
-        <v>134</v>
-      </c>
-      <c r="G11" t="s">
-        <v>133</v>
-      </c>
-      <c r="H11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I11" t="s">
-        <v>134</v>
-      </c>
-      <c r="J11" t="s">
-        <v>133</v>
-      </c>
-      <c r="K11" t="s">
-        <v>133</v>
-      </c>
-      <c r="M11" t="s">
-        <v>134</v>
-      </c>
-      <c r="N11" t="s">
-        <v>134</v>
-      </c>
-      <c r="O11" t="s">
-        <v>133</v>
-      </c>
-      <c r="P11" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>135</v>
-      </c>
-      <c r="E12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G12" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" t="s">
-        <v>133</v>
-      </c>
-      <c r="I12" t="s">
-        <v>134</v>
-      </c>
-      <c r="J12" t="s">
-        <v>133</v>
-      </c>
-      <c r="M12" t="s">
-        <v>134</v>
-      </c>
-      <c r="N12" t="s">
-        <v>134</v>
-      </c>
-      <c r="O12" t="s">
-        <v>133</v>
-      </c>
-      <c r="P12" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>138</v>
-      </c>
-      <c r="E13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F13" t="s">
-        <v>134</v>
-      </c>
-      <c r="G13" t="s">
-        <v>134</v>
-      </c>
-      <c r="H13" t="s">
-        <v>134</v>
-      </c>
-      <c r="I13" t="s">
-        <v>133</v>
-      </c>
-      <c r="J13" t="s">
-        <v>133</v>
-      </c>
-      <c r="K13" t="s">
-        <v>134</v>
-      </c>
-      <c r="M13" t="s">
-        <v>134</v>
-      </c>
-      <c r="N13" t="s">
-        <v>134</v>
-      </c>
-      <c r="O13" t="s">
-        <v>134</v>
-      </c>
-      <c r="P13" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>139</v>
-      </c>
-      <c r="E14" t="s">
-        <v>134</v>
-      </c>
-      <c r="F14" t="s">
-        <v>134</v>
-      </c>
-      <c r="G14" t="s">
-        <v>133</v>
-      </c>
-      <c r="H14" t="s">
-        <v>133</v>
-      </c>
-      <c r="I14" t="s">
-        <v>133</v>
-      </c>
-      <c r="J14" t="s">
-        <v>133</v>
-      </c>
-      <c r="M14" t="s">
-        <v>133</v>
-      </c>
-      <c r="N14" t="s">
-        <v>134</v>
-      </c>
-      <c r="O14" t="s">
-        <v>133</v>
-      </c>
-      <c r="P14" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F15" t="s">
-        <v>134</v>
-      </c>
-      <c r="G15" t="s">
-        <v>133</v>
-      </c>
-      <c r="H15" t="s">
-        <v>133</v>
-      </c>
-      <c r="I15" t="s">
-        <v>134</v>
-      </c>
-      <c r="J15" t="s">
-        <v>134</v>
-      </c>
-      <c r="K15" t="s">
-        <v>133</v>
-      </c>
-      <c r="L15" t="s">
-        <v>134</v>
-      </c>
-      <c r="M15" t="s">
-        <v>134</v>
-      </c>
-      <c r="N15" t="s">
-        <v>134</v>
-      </c>
-      <c r="O15" t="s">
-        <v>133</v>
-      </c>
-      <c r="P15" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>143</v>
-      </c>
-      <c r="E16" t="s">
-        <v>134</v>
-      </c>
-      <c r="F16" t="s">
-        <v>134</v>
-      </c>
-      <c r="G16" t="s">
-        <v>133</v>
-      </c>
-      <c r="H16" t="s">
-        <v>133</v>
-      </c>
-      <c r="I16" t="s">
-        <v>134</v>
-      </c>
-      <c r="J16" t="s">
-        <v>133</v>
-      </c>
-      <c r="K16" t="s">
-        <v>134</v>
-      </c>
-      <c r="L16" t="s">
-        <v>133</v>
-      </c>
-      <c r="M16" t="s">
-        <v>134</v>
-      </c>
-      <c r="N16" t="s">
-        <v>134</v>
-      </c>
-      <c r="O16" t="s">
-        <v>134</v>
-      </c>
-      <c r="P16" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17" t="s">
-        <v>134</v>
-      </c>
-      <c r="F17" t="s">
-        <v>133</v>
-      </c>
-      <c r="G17" t="s">
-        <v>134</v>
-      </c>
-      <c r="H17" t="s">
-        <v>134</v>
-      </c>
-      <c r="I17" t="s">
-        <v>134</v>
-      </c>
-      <c r="J17" t="s">
-        <v>133</v>
-      </c>
-      <c r="K17" t="s">
-        <v>134</v>
-      </c>
-      <c r="L17" t="s">
-        <v>134</v>
-      </c>
-      <c r="M17" t="s">
-        <v>133</v>
-      </c>
-      <c r="N17" t="s">
-        <v>134</v>
-      </c>
-      <c r="O17" t="s">
-        <v>134</v>
-      </c>
-      <c r="P17" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" t="s">
-        <v>134</v>
-      </c>
-      <c r="F18" t="s">
-        <v>134</v>
-      </c>
-      <c r="G18" t="s">
-        <v>134</v>
-      </c>
-      <c r="H18" t="s">
-        <v>134</v>
-      </c>
-      <c r="I18" t="s">
-        <v>134</v>
-      </c>
-      <c r="J18" t="s">
-        <v>134</v>
-      </c>
-      <c r="K18" t="s">
-        <v>134</v>
-      </c>
-      <c r="L18" t="s">
-        <v>134</v>
-      </c>
-      <c r="M18" t="s">
-        <v>134</v>
-      </c>
-      <c r="N18" t="s">
-        <v>133</v>
-      </c>
-      <c r="O18" t="s">
-        <v>134</v>
-      </c>
-      <c r="P18" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" t="s">
-        <v>134</v>
-      </c>
-      <c r="F19" t="s">
-        <v>134</v>
-      </c>
-      <c r="G19" t="s">
-        <v>133</v>
-      </c>
-      <c r="H19" t="s">
-        <v>133</v>
-      </c>
-      <c r="I19" t="s">
-        <v>134</v>
-      </c>
-      <c r="J19" t="s">
-        <v>133</v>
-      </c>
-      <c r="K19" t="s">
-        <v>133</v>
-      </c>
-      <c r="L19" t="s">
-        <v>134</v>
-      </c>
-      <c r="M19" t="s">
-        <v>134</v>
-      </c>
-      <c r="N19" t="s">
-        <v>134</v>
-      </c>
-      <c r="O19" t="s">
-        <v>133</v>
-      </c>
-      <c r="P19" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" t="s">
-        <v>133</v>
-      </c>
-      <c r="F20" t="s">
-        <v>134</v>
-      </c>
-      <c r="G20" t="s">
-        <v>133</v>
-      </c>
-      <c r="H20" t="s">
-        <v>133</v>
-      </c>
-      <c r="I20" t="s">
-        <v>134</v>
-      </c>
-      <c r="J20" t="s">
-        <v>133</v>
-      </c>
-      <c r="K20" t="s">
-        <v>133</v>
-      </c>
-      <c r="L20" t="s">
-        <v>133</v>
-      </c>
-      <c r="M20" t="s">
-        <v>134</v>
-      </c>
-      <c r="N20" t="s">
-        <v>134</v>
-      </c>
-      <c r="O20" t="s">
-        <v>133</v>
-      </c>
-      <c r="P20" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>148</v>
-      </c>
-      <c r="E21" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" t="s">
-        <v>134</v>
-      </c>
-      <c r="G21" t="s">
-        <v>133</v>
-      </c>
-      <c r="H21" t="s">
-        <v>133</v>
-      </c>
-      <c r="I21" t="s">
-        <v>134</v>
-      </c>
-      <c r="J21" t="s">
-        <v>133</v>
-      </c>
-      <c r="K21" t="s">
-        <v>133</v>
-      </c>
-      <c r="L21" t="s">
-        <v>133</v>
-      </c>
-      <c r="M21" t="s">
-        <v>134</v>
-      </c>
-      <c r="N21" t="s">
-        <v>134</v>
-      </c>
-      <c r="O21" t="s">
-        <v>133</v>
-      </c>
-      <c r="P21" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" t="s">
-        <v>134</v>
-      </c>
-      <c r="F22" t="s">
-        <v>134</v>
-      </c>
-      <c r="G22" t="s">
-        <v>133</v>
-      </c>
-      <c r="H22" t="s">
-        <v>133</v>
-      </c>
-      <c r="I22" t="s">
-        <v>134</v>
-      </c>
-      <c r="J22" t="s">
-        <v>133</v>
-      </c>
-      <c r="K22" t="s">
-        <v>133</v>
-      </c>
-      <c r="L22" t="s">
-        <v>133</v>
-      </c>
-      <c r="M22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N22" t="s">
-        <v>134</v>
-      </c>
-      <c r="O22" t="s">
-        <v>133</v>
-      </c>
-      <c r="P22" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>133</v>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Carica livelli solo filtrati (leggermente più veloce)
</commit_message>
<xml_diff>
--- a/Analisi approfondita sovrapponibili.xlsx
+++ b/Analisi approfondita sovrapponibili.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documenti\repositories\Super Mario Deep Maker 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599F3DFF-8C44-4EE7-ADA3-E377629A17CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1395C22A-E655-4414-98BE-FDB7BF6B5D7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,7 +530,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -609,6 +609,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFCFCF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB0B0B0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8E8E8E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -622,22 +652,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -646,11 +688,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF808080"/>
+      <color rgb="FF8E8E8E"/>
+      <color rgb="FF9B9B9B"/>
+      <color rgb="FF999999"/>
+      <color rgb="FFB0B0B0"/>
+      <color rgb="FFCFCFCF"/>
+      <color rgb="FF6D6D6D"/>
       <color rgb="FFB9FFFF"/>
       <color rgb="FFF9ADAD"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFCCF20E"/>
-      <color rgb="FFFDA9F9"/>
     </mruColors>
   </colors>
   <extLst>
@@ -4333,10 +4380,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76425061-D43B-44F5-ADB3-D0ABE7860380}">
-  <dimension ref="B8:T43"/>
+  <dimension ref="B2:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4349,1227 +4396,1228 @@
     <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.28515625" customWidth="1"/>
     <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" customWidth="1"/>
     <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T4" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S6" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T7" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="C8" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R8" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S8" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T8" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="C9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="P9" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T9" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="C10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T10" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="C11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T11" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="C12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S12" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T12" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q8" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="S8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="T8" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" t="s">
-        <v>134</v>
-      </c>
-      <c r="F9" t="s">
-        <v>134</v>
-      </c>
-      <c r="G9" t="s">
-        <v>134</v>
-      </c>
-      <c r="H9" t="s">
-        <v>134</v>
-      </c>
-      <c r="I9" t="s">
-        <v>134</v>
-      </c>
-      <c r="J9" t="s">
-        <v>134</v>
-      </c>
-      <c r="K9" t="s">
-        <v>134</v>
-      </c>
-      <c r="L9" t="s">
-        <v>134</v>
-      </c>
-      <c r="M9" t="s">
-        <v>134</v>
-      </c>
-      <c r="N9" t="s">
-        <v>133</v>
-      </c>
-      <c r="O9" t="s">
-        <v>133</v>
-      </c>
-      <c r="P9" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>134</v>
-      </c>
-      <c r="R9" t="s">
-        <v>134</v>
-      </c>
-      <c r="S9" t="s">
-        <v>134</v>
-      </c>
-      <c r="T9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" t="s">
-        <v>134</v>
-      </c>
-      <c r="G10" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" t="s">
-        <v>134</v>
-      </c>
-      <c r="I10" t="s">
-        <v>134</v>
-      </c>
-      <c r="J10" t="s">
-        <v>134</v>
-      </c>
-      <c r="K10" t="s">
-        <v>133</v>
-      </c>
-      <c r="L10" t="s">
-        <v>134</v>
-      </c>
-      <c r="M10" t="s">
-        <v>134</v>
-      </c>
-      <c r="N10" t="s">
-        <v>134</v>
-      </c>
-      <c r="O10" t="s">
-        <v>134</v>
-      </c>
-      <c r="P10" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>134</v>
-      </c>
-      <c r="R10" t="s">
-        <v>134</v>
-      </c>
-      <c r="S10" t="s">
-        <v>134</v>
-      </c>
-      <c r="T10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F11" t="s">
-        <v>133</v>
-      </c>
-      <c r="G11" t="s">
-        <v>134</v>
-      </c>
-      <c r="H11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I11" t="s">
-        <v>133</v>
-      </c>
-      <c r="J11" t="s">
-        <v>133</v>
-      </c>
-      <c r="K11" t="s">
-        <v>134</v>
-      </c>
-      <c r="L11" t="s">
-        <v>134</v>
-      </c>
-      <c r="M11" t="s">
-        <v>133</v>
-      </c>
-      <c r="N11" t="s">
-        <v>133</v>
-      </c>
-      <c r="O11" t="s">
-        <v>133</v>
-      </c>
-      <c r="P11" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>134</v>
-      </c>
-      <c r="R11" t="s">
-        <v>134</v>
-      </c>
-      <c r="S11" t="s">
-        <v>134</v>
-      </c>
-      <c r="T11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E12" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G12" t="s">
-        <v>134</v>
-      </c>
-      <c r="H12" t="s">
-        <v>133</v>
-      </c>
-      <c r="I12" t="s">
-        <v>133</v>
-      </c>
-      <c r="J12" t="s">
-        <v>133</v>
-      </c>
-      <c r="K12" t="s">
-        <v>134</v>
-      </c>
-      <c r="L12" t="s">
-        <v>134</v>
-      </c>
-      <c r="M12" t="s">
-        <v>133</v>
-      </c>
-      <c r="N12" t="s">
-        <v>133</v>
-      </c>
-      <c r="O12" t="s">
-        <v>133</v>
-      </c>
-      <c r="P12" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>134</v>
-      </c>
-      <c r="R12" t="s">
-        <v>134</v>
-      </c>
-      <c r="S12" t="s">
-        <v>134</v>
-      </c>
-      <c r="T12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F13" t="s">
-        <v>134</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="H13" t="s">
-        <v>133</v>
-      </c>
-      <c r="I13" t="s">
-        <v>134</v>
-      </c>
-      <c r="J13" t="s">
-        <v>134</v>
-      </c>
-      <c r="K13" t="s">
-        <v>134</v>
-      </c>
-      <c r="L13" t="s">
-        <v>134</v>
-      </c>
-      <c r="M13" t="s">
-        <v>134</v>
-      </c>
-      <c r="N13" t="s">
-        <v>134</v>
-      </c>
-      <c r="O13" t="s">
-        <v>134</v>
-      </c>
-      <c r="P13" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>134</v>
-      </c>
-      <c r="R13" t="s">
-        <v>134</v>
-      </c>
-      <c r="S13" t="s">
-        <v>134</v>
-      </c>
-      <c r="T13" t="s">
+      <c r="C13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T13" s="19" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" t="s">
-        <v>134</v>
-      </c>
-      <c r="E14" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" t="s">
-        <v>133</v>
-      </c>
-      <c r="G14" t="s">
-        <v>133</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="I14" t="s">
-        <v>134</v>
-      </c>
-      <c r="J14" t="s">
-        <v>133</v>
-      </c>
-      <c r="K14" t="s">
-        <v>133</v>
-      </c>
-      <c r="L14" t="s">
-        <v>134</v>
-      </c>
-      <c r="M14" t="s">
-        <v>133</v>
-      </c>
-      <c r="N14" t="s">
-        <v>133</v>
-      </c>
-      <c r="O14" t="s">
-        <v>134</v>
-      </c>
-      <c r="P14" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>134</v>
-      </c>
-      <c r="R14" t="s">
-        <v>134</v>
-      </c>
-      <c r="S14" t="s">
-        <v>134</v>
-      </c>
-      <c r="T14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q14" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S14" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T14" s="19" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15" t="s">
-        <v>134</v>
-      </c>
-      <c r="D15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E15" t="s">
-        <v>133</v>
-      </c>
-      <c r="F15" t="s">
-        <v>133</v>
-      </c>
-      <c r="G15" t="s">
-        <v>134</v>
-      </c>
-      <c r="H15" t="s">
-        <v>134</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J15" t="s">
-        <v>134</v>
-      </c>
-      <c r="K15" t="s">
-        <v>134</v>
-      </c>
-      <c r="L15" t="s">
-        <v>134</v>
-      </c>
-      <c r="M15" t="s">
-        <v>133</v>
-      </c>
-      <c r="N15" t="s">
-        <v>133</v>
-      </c>
-      <c r="O15" t="s">
-        <v>133</v>
-      </c>
-      <c r="P15" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>134</v>
-      </c>
-      <c r="R15" t="s">
-        <v>134</v>
-      </c>
-      <c r="S15" t="s">
-        <v>134</v>
-      </c>
-      <c r="T15" t="s">
+      <c r="B15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O15" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T15" s="19" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E16" t="s">
-        <v>133</v>
-      </c>
-      <c r="F16" t="s">
-        <v>133</v>
-      </c>
-      <c r="G16" t="s">
-        <v>134</v>
-      </c>
-      <c r="H16" t="s">
-        <v>133</v>
-      </c>
-      <c r="I16" t="s">
-        <v>134</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="K16" t="s">
-        <v>134</v>
-      </c>
-      <c r="L16" t="s">
-        <v>134</v>
-      </c>
-      <c r="M16" t="s">
-        <v>134</v>
-      </c>
-      <c r="N16" t="s">
-        <v>133</v>
-      </c>
-      <c r="O16" t="s">
-        <v>133</v>
-      </c>
-      <c r="P16" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>134</v>
-      </c>
-      <c r="R16" t="s">
-        <v>134</v>
-      </c>
-      <c r="S16" t="s">
-        <v>134</v>
-      </c>
-      <c r="T16" t="s">
+      <c r="B16" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M16" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O16" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="P16" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q16" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R16" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S16" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T16" s="19" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E17" t="s">
-        <v>134</v>
-      </c>
-      <c r="F17" t="s">
-        <v>134</v>
-      </c>
-      <c r="G17" t="s">
-        <v>134</v>
-      </c>
-      <c r="H17" t="s">
-        <v>133</v>
-      </c>
-      <c r="I17" t="s">
-        <v>134</v>
-      </c>
-      <c r="J17" t="s">
-        <v>134</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="L17" t="s">
-        <v>134</v>
-      </c>
-      <c r="M17" t="s">
-        <v>134</v>
-      </c>
-      <c r="N17" t="s">
-        <v>133</v>
-      </c>
-      <c r="O17" t="s">
-        <v>134</v>
-      </c>
-      <c r="P17" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>134</v>
-      </c>
-      <c r="R17" t="s">
-        <v>134</v>
-      </c>
-      <c r="S17" t="s">
-        <v>134</v>
-      </c>
-      <c r="T17" t="s">
+      <c r="B17" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q17" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="R17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T17" s="19" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" t="s">
-        <v>134</v>
-      </c>
-      <c r="E18" t="s">
-        <v>134</v>
-      </c>
-      <c r="F18" t="s">
-        <v>134</v>
-      </c>
-      <c r="G18" t="s">
-        <v>134</v>
-      </c>
-      <c r="H18" t="s">
-        <v>134</v>
-      </c>
-      <c r="I18" t="s">
-        <v>134</v>
-      </c>
-      <c r="J18" t="s">
-        <v>134</v>
-      </c>
-      <c r="K18" t="s">
-        <v>134</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="M18" t="s">
-        <v>134</v>
-      </c>
-      <c r="N18" t="s">
-        <v>134</v>
-      </c>
-      <c r="O18" t="s">
-        <v>134</v>
-      </c>
-      <c r="P18" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>134</v>
-      </c>
-      <c r="R18" t="s">
-        <v>134</v>
-      </c>
-      <c r="S18" t="s">
-        <v>134</v>
-      </c>
-      <c r="T18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R18" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="S18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T18" s="19" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" t="s">
-        <v>133</v>
-      </c>
-      <c r="F19" t="s">
-        <v>133</v>
-      </c>
-      <c r="G19" t="s">
-        <v>134</v>
-      </c>
-      <c r="H19" t="s">
-        <v>133</v>
-      </c>
-      <c r="I19" t="s">
-        <v>133</v>
-      </c>
-      <c r="J19" t="s">
-        <v>134</v>
-      </c>
-      <c r="K19" t="s">
-        <v>134</v>
-      </c>
-      <c r="L19" t="s">
-        <v>134</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="N19" t="s">
-        <v>134</v>
-      </c>
-      <c r="O19" t="s">
-        <v>133</v>
-      </c>
-      <c r="P19" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>134</v>
-      </c>
-      <c r="R19" t="s">
-        <v>134</v>
-      </c>
-      <c r="S19" t="s">
-        <v>134</v>
-      </c>
-      <c r="T19" t="s">
+      <c r="B19" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S19" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="T19" s="19" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" t="s">
-        <v>133</v>
-      </c>
-      <c r="D20" t="s">
-        <v>134</v>
-      </c>
-      <c r="E20" t="s">
-        <v>133</v>
-      </c>
-      <c r="F20" t="s">
-        <v>133</v>
-      </c>
-      <c r="G20" t="s">
-        <v>134</v>
-      </c>
-      <c r="H20" t="s">
-        <v>133</v>
-      </c>
-      <c r="I20" t="s">
-        <v>133</v>
-      </c>
-      <c r="J20" t="s">
-        <v>133</v>
-      </c>
-      <c r="K20" t="s">
-        <v>134</v>
-      </c>
-      <c r="L20" t="s">
-        <v>134</v>
-      </c>
-      <c r="M20" t="s">
-        <v>133</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="O20" t="s">
-        <v>133</v>
-      </c>
-      <c r="P20" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>134</v>
-      </c>
-      <c r="R20" t="s">
-        <v>134</v>
-      </c>
-      <c r="S20" t="s">
-        <v>134</v>
-      </c>
-      <c r="T20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21" t="s">
-        <v>134</v>
-      </c>
-      <c r="E21" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" t="s">
-        <v>133</v>
-      </c>
-      <c r="G21" t="s">
-        <v>134</v>
-      </c>
-      <c r="H21" t="s">
-        <v>133</v>
-      </c>
-      <c r="I21" t="s">
-        <v>133</v>
-      </c>
-      <c r="J21" t="s">
-        <v>133</v>
-      </c>
-      <c r="K21" t="s">
-        <v>134</v>
-      </c>
-      <c r="L21" t="s">
-        <v>134</v>
-      </c>
-      <c r="M21" t="s">
-        <v>133</v>
-      </c>
-      <c r="N21" t="s">
-        <v>133</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="P21" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>134</v>
-      </c>
-      <c r="R21" t="s">
-        <v>134</v>
-      </c>
-      <c r="S21" t="s">
-        <v>134</v>
-      </c>
-      <c r="T21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" t="s">
-        <v>133</v>
-      </c>
-      <c r="D22" t="s">
-        <v>134</v>
-      </c>
-      <c r="E22" t="s">
-        <v>133</v>
-      </c>
-      <c r="F22" t="s">
-        <v>133</v>
-      </c>
-      <c r="G22" t="s">
-        <v>134</v>
-      </c>
-      <c r="H22" t="s">
-        <v>133</v>
-      </c>
-      <c r="I22" t="s">
-        <v>133</v>
-      </c>
-      <c r="J22" t="s">
-        <v>134</v>
-      </c>
-      <c r="K22" t="s">
-        <v>134</v>
-      </c>
-      <c r="L22" t="s">
-        <v>134</v>
-      </c>
-      <c r="M22" t="s">
-        <v>133</v>
-      </c>
-      <c r="N22" t="s">
-        <v>133</v>
-      </c>
-      <c r="O22" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="P22" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>134</v>
-      </c>
-      <c r="R22" t="s">
-        <v>134</v>
-      </c>
-      <c r="S22" t="s">
-        <v>134</v>
-      </c>
-      <c r="T22" t="s">
-        <v>134</v>
+      <c r="B20" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="N20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T20" s="18" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" t="s">
-        <v>134</v>
-      </c>
-      <c r="E23" t="s">
-        <v>134</v>
-      </c>
-      <c r="F23" t="s">
-        <v>134</v>
-      </c>
-      <c r="G23" t="s">
-        <v>134</v>
-      </c>
-      <c r="H23" t="s">
-        <v>134</v>
-      </c>
-      <c r="I23" t="s">
-        <v>134</v>
-      </c>
-      <c r="J23" t="s">
-        <v>134</v>
-      </c>
-      <c r="K23" t="s">
-        <v>134</v>
-      </c>
-      <c r="L23" t="s">
-        <v>134</v>
-      </c>
-      <c r="M23" t="s">
-        <v>134</v>
-      </c>
-      <c r="N23" t="s">
-        <v>134</v>
-      </c>
-      <c r="O23" t="s">
-        <v>134</v>
-      </c>
-      <c r="P23" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q23" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="R23" t="s">
-        <v>134</v>
-      </c>
-      <c r="S23" t="s">
-        <v>134</v>
-      </c>
-      <c r="T23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C24" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" t="s">
-        <v>134</v>
-      </c>
-      <c r="E24" t="s">
-        <v>134</v>
-      </c>
-      <c r="F24" t="s">
-        <v>134</v>
-      </c>
-      <c r="G24" t="s">
-        <v>134</v>
-      </c>
-      <c r="H24" t="s">
-        <v>134</v>
-      </c>
-      <c r="I24" t="s">
-        <v>134</v>
-      </c>
-      <c r="J24" t="s">
-        <v>134</v>
-      </c>
-      <c r="K24" t="s">
-        <v>134</v>
-      </c>
-      <c r="L24" t="s">
-        <v>134</v>
-      </c>
-      <c r="M24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N24" t="s">
-        <v>134</v>
-      </c>
-      <c r="O24" t="s">
-        <v>134</v>
-      </c>
-      <c r="P24" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>134</v>
-      </c>
-      <c r="R24" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="S24" t="s">
-        <v>134</v>
-      </c>
-      <c r="T24" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="C25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D25" t="s">
-        <v>134</v>
-      </c>
-      <c r="E25" t="s">
-        <v>134</v>
-      </c>
-      <c r="F25" t="s">
-        <v>134</v>
-      </c>
-      <c r="G25" t="s">
-        <v>134</v>
-      </c>
-      <c r="H25" t="s">
-        <v>134</v>
-      </c>
-      <c r="I25" t="s">
-        <v>134</v>
-      </c>
-      <c r="J25" t="s">
-        <v>134</v>
-      </c>
-      <c r="K25" t="s">
-        <v>134</v>
-      </c>
-      <c r="L25" t="s">
-        <v>134</v>
-      </c>
-      <c r="M25" t="s">
-        <v>134</v>
-      </c>
-      <c r="N25" t="s">
-        <v>134</v>
-      </c>
-      <c r="O25" t="s">
-        <v>134</v>
-      </c>
-      <c r="P25" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>134</v>
-      </c>
-      <c r="R25" t="s">
-        <v>134</v>
-      </c>
-      <c r="S25" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="T25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C26" t="s">
-        <v>134</v>
-      </c>
-      <c r="D26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E26" t="s">
-        <v>134</v>
-      </c>
-      <c r="F26" t="s">
-        <v>134</v>
-      </c>
-      <c r="G26" t="s">
-        <v>134</v>
-      </c>
-      <c r="H26" t="s">
-        <v>134</v>
-      </c>
-      <c r="I26" t="s">
-        <v>134</v>
-      </c>
-      <c r="J26" t="s">
-        <v>134</v>
-      </c>
-      <c r="K26" t="s">
-        <v>134</v>
-      </c>
-      <c r="L26" t="s">
-        <v>134</v>
-      </c>
-      <c r="M26" t="s">
-        <v>134</v>
-      </c>
-      <c r="N26" t="s">
-        <v>134</v>
-      </c>
-      <c r="O26" t="s">
-        <v>134</v>
-      </c>
-      <c r="P26" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>134</v>
-      </c>
-      <c r="R26" t="s">
-        <v>134</v>
-      </c>
-      <c r="S26" t="s">
-        <v>134</v>
-      </c>
-      <c r="T26" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C30" s="7" t="s">
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B31" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inizio fine livelli e altri strati
</commit_message>
<xml_diff>
--- a/Analisi approfondita sovrapponibili.xlsx
+++ b/Analisi approfondita sovrapponibili.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documenti\repositories\Super Mario Deep Maker 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AE6EF8-87EC-4D4B-BA31-53EFC44CBBE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CFB459-9246-4C05-B137-A47453E3C68C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Foglio4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$L$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$L$128</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1012,11 +1012,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:S128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G124" sqref="G124"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1085,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1098,7 +1099,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1126,7 +1127,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1140,7 +1141,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1170,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1211,7 +1212,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1275,7 +1276,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1289,7 +1290,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1303,7 +1304,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1317,7 +1318,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1331,7 +1332,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1345,7 +1346,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1359,7 +1360,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1373,7 +1374,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1433,7 +1434,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1447,7 +1448,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1489,7 +1490,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1503,7 +1504,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1517,7 +1518,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1528,7 +1529,7 @@
         <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="E28" t="s">
         <v>128</v>
@@ -1552,7 +1553,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1601,7 +1602,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1643,7 +1644,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1671,7 +1672,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -1699,7 +1700,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1716,7 +1717,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>44</v>
       </c>
       <c r="D39" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="E39" t="s">
         <v>128</v>
@@ -1754,7 +1755,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -1792,7 +1793,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1806,7 +1807,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1820,7 +1821,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1834,7 +1835,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1848,7 +1849,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1862,7 +1863,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -1876,7 +1877,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -1890,7 +1891,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1904,7 +1905,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -1918,7 +1919,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -1932,7 +1933,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1960,7 +1961,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1988,7 +1989,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -2002,7 +2003,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2016,7 +2017,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -2057,7 +2058,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -2085,7 +2086,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -2099,7 +2100,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -2113,7 +2114,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -2127,7 +2128,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -2141,7 +2142,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -2155,7 +2156,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -2169,7 +2170,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -2211,7 +2212,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -2225,7 +2226,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -2266,7 +2267,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>33</v>
       </c>
@@ -2280,7 +2281,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -2294,7 +2295,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -2308,7 +2309,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -2322,7 +2323,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>33</v>
       </c>
@@ -2336,7 +2337,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -2350,7 +2351,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>33</v>
       </c>
@@ -2364,7 +2365,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -2378,7 +2379,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -2392,7 +2393,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -2420,7 +2421,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -2434,7 +2435,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>33</v>
       </c>
@@ -2448,7 +2449,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -2476,7 +2477,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -2490,7 +2491,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -2504,7 +2505,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -2579,7 +2580,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>33</v>
       </c>
@@ -2593,7 +2594,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -2637,7 +2638,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -2651,7 +2652,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -2695,7 +2696,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -2723,7 +2724,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -2743,7 +2744,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>3</v>
       </c>
@@ -2757,7 +2758,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -2771,7 +2772,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>3</v>
       </c>
@@ -2785,7 +2786,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -2799,7 +2800,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -2813,7 +2814,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>33</v>
       </c>
@@ -2827,7 +2828,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>3</v>
       </c>
@@ -2841,7 +2842,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>3</v>
       </c>
@@ -2855,7 +2856,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -2883,7 +2884,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -2897,7 +2898,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>3</v>
       </c>
@@ -2911,7 +2912,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -2925,7 +2926,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>33</v>
       </c>
@@ -2939,7 +2940,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -2953,7 +2954,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>33</v>
       </c>
@@ -2967,7 +2968,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>16</v>
       </c>
@@ -2981,7 +2982,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>16</v>
       </c>
@@ -2995,7 +2996,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>3</v>
       </c>
@@ -3009,7 +3010,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -3023,7 +3024,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -3037,7 +3038,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>3</v>
       </c>
@@ -3051,7 +3052,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>16</v>
       </c>
@@ -3065,7 +3066,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>119</v>
       </c>
@@ -3076,7 +3077,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>120</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>121</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>122</v>
       </c>
@@ -3109,7 +3110,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>123</v>
       </c>
@@ -3120,7 +3121,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>124</v>
       </c>
@@ -3131,7 +3132,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>125</v>
       </c>
@@ -3142,7 +3143,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>126</v>
       </c>
@@ -3154,7 +3155,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L121" xr:uid="{AF469F71-5011-4551-9995-E4BE0EFC6196}"/>
+  <autoFilter ref="A1:L128" xr:uid="{AF469F71-5011-4551-9995-E4BE0EFC6196}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Terreno"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4539,7 +4546,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Snake e altri fix
</commit_message>
<xml_diff>
--- a/Analisi approfondita sovrapponibili.xlsx
+++ b/Analisi approfondita sovrapponibili.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documenti\repositories\Super Mario Deep Maker 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80497FB-BD61-4B6D-BCC3-3382E1F31251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8081782E-50E6-4654-9956-5AB9EF17B919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19245" yWindow="3810" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="2790" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Foglio6" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$M$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$M$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="163">
   <si>
     <t>Nome</t>
   </si>
@@ -527,6 +527,9 @@
   </si>
   <si>
     <t>T contraria</t>
+  </si>
+  <si>
+    <t>snakeTrack</t>
   </si>
 </sst>
 </file>
@@ -1032,11 +1035,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T128"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:T129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D122" sqref="D122:D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1112,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1125,7 +1129,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1142,7 +1146,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1159,7 +1163,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1176,7 +1180,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1212,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1225,7 +1229,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1242,7 +1246,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1259,7 +1263,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1291,7 +1295,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1329,7 +1333,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1346,7 +1350,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1363,7 +1367,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1380,7 +1384,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1397,7 +1401,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1414,7 +1418,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1431,7 +1435,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1448,7 +1452,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1483,7 +1487,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1500,7 +1504,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1517,7 +1521,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1551,7 +1555,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1568,7 +1572,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1585,7 +1589,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1602,7 +1606,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1619,7 +1623,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1657,7 +1661,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1695,7 +1699,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1712,7 +1716,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1729,7 +1733,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1746,7 +1750,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1763,7 +1767,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1780,7 +1784,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1797,7 +1801,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -1814,7 +1818,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -1831,7 +1835,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1851,7 +1855,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1892,7 +1896,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -1933,7 +1937,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1950,7 +1954,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1967,7 +1971,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -2001,7 +2005,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2018,7 +2022,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2035,7 +2039,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -2052,7 +2056,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -2069,7 +2073,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -2086,7 +2090,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -2103,7 +2107,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -2120,7 +2124,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -2137,7 +2141,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -2154,7 +2158,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -2171,7 +2175,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -2188,7 +2192,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2205,7 +2209,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -2249,7 +2253,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -2266,7 +2270,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -2283,7 +2287,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -2300,7 +2304,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -2317,7 +2321,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -2334,7 +2338,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -2351,7 +2355,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -2368,7 +2372,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -2385,7 +2389,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -2402,7 +2406,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -2419,7 +2423,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -2436,7 +2440,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -2453,7 +2457,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -2497,7 +2501,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>33</v>
       </c>
@@ -2514,7 +2518,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -2531,7 +2535,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -2548,7 +2552,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -2565,7 +2569,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>33</v>
       </c>
@@ -2582,7 +2586,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -2599,7 +2603,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>33</v>
       </c>
@@ -2616,7 +2620,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -2633,7 +2637,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -2650,7 +2654,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -2667,7 +2671,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -2684,7 +2688,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -2701,7 +2705,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>33</v>
       </c>
@@ -2718,7 +2722,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -2735,7 +2739,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -2769,7 +2773,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -2786,7 +2790,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -2803,7 +2807,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -2853,7 +2857,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -2870,7 +2874,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>33</v>
       </c>
@@ -2887,7 +2891,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -2934,7 +2938,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -2951,7 +2955,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -2998,7 +3002,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -3015,7 +3019,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -3032,7 +3036,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -3055,7 +3059,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>3</v>
       </c>
@@ -3072,7 +3076,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -3089,7 +3093,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>3</v>
       </c>
@@ -3106,7 +3110,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -3123,7 +3127,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -3140,7 +3144,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>33</v>
       </c>
@@ -3157,7 +3161,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>3</v>
       </c>
@@ -3174,7 +3178,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>3</v>
       </c>
@@ -3191,7 +3195,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -3208,7 +3212,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -3225,7 +3229,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -3242,7 +3246,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>3</v>
       </c>
@@ -3259,7 +3263,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -3276,7 +3280,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>33</v>
       </c>
@@ -3293,7 +3297,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -3310,7 +3314,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>33</v>
       </c>
@@ -3327,7 +3331,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>16</v>
       </c>
@@ -3344,7 +3348,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>16</v>
       </c>
@@ -3361,7 +3365,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>3</v>
       </c>
@@ -3378,7 +3382,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -3395,7 +3399,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -3412,7 +3416,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>3</v>
       </c>
@@ -3429,7 +3433,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>16</v>
       </c>
@@ -3446,7 +3450,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>119</v>
       </c>
@@ -3460,7 +3464,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>120</v>
       </c>
@@ -3474,7 +3478,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>121</v>
       </c>
@@ -3488,7 +3492,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>122</v>
       </c>
@@ -3502,7 +3506,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>123</v>
       </c>
@@ -3516,7 +3520,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>124</v>
       </c>
@@ -3530,7 +3534,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>125</v>
       </c>
@@ -3544,7 +3548,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>126</v>
       </c>
@@ -3558,8 +3562,28 @@
         <v>157</v>
       </c>
     </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>127</v>
+      </c>
+      <c r="C129" t="s">
+        <v>162</v>
+      </c>
+      <c r="D129" t="s">
+        <v>141</v>
+      </c>
+      <c r="E129" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M128" xr:uid="{AF469F71-5011-4551-9995-E4BE0EFC6196}"/>
+  <autoFilter ref="A1:M129" xr:uid="{AF469F71-5011-4551-9995-E4BE0EFC6196}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Snake"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4943,8 +4967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{173310C4-1295-4648-B14B-887801CC320C}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5151,10 +5175,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E01B41-BDA6-4A71-AD93-F66AD7291B52}">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C128"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6602,6 +6626,102 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>135</v>
+      </c>
+      <c r="C121">
+        <f>VLOOKUP(B121,Foglio2!$A$1:$B$21,2,)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>135</v>
+      </c>
+      <c r="C122">
+        <f>VLOOKUP(B122,Foglio2!$A$1:$B$21,2,)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>135</v>
+      </c>
+      <c r="C123">
+        <f>VLOOKUP(B123,Foglio2!$A$1:$B$21,2,)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>135</v>
+      </c>
+      <c r="C124">
+        <f>VLOOKUP(B124,Foglio2!$A$1:$B$21,2,)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>135</v>
+      </c>
+      <c r="C125">
+        <f>VLOOKUP(B125,Foglio2!$A$1:$B$21,2,)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>135</v>
+      </c>
+      <c r="C126">
+        <f>VLOOKUP(B126,Foglio2!$A$1:$B$21,2,)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>135</v>
+      </c>
+      <c r="C127">
+        <f>VLOOKUP(B127,Foglio2!$A$1:$B$21,2,)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>141</v>
+      </c>
+      <c r="C128">
+        <f>VLOOKUP(B128,Foglio2!$A$1:$B$21,2,)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6609,10 +6729,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFB9E16-775B-45A9-8343-00B87C17FFBF}">
-  <dimension ref="B1:R128"/>
+  <dimension ref="B1:R129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="G116" sqref="G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7443,7 +7563,7 @@
         <v>157</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D128" si="1">VLOOKUP(C67,$Q$2:$R$6,2, FALSE)</f>
+        <f t="shared" ref="D67:D129" si="1">VLOOKUP(C67,$Q$2:$R$6,2, FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -8175,6 +8295,18 @@
         <v>157</v>
       </c>
       <c r="D128">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>127</v>
+      </c>
+      <c r="C129" t="s">
+        <v>157</v>
+      </c>
+      <c r="D129">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8186,10 +8318,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C226AE5-74AD-41B9-AE4D-1426914045ED}">
-  <dimension ref="A2:B128"/>
+  <dimension ref="A2:B129"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B128"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9210,6 +9342,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
gentle fix per davvero
</commit_message>
<xml_diff>
--- a/Analisi approfondita sovrapponibili.xlsx
+++ b/Analisi approfondita sovrapponibili.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documenti\repositories\Super Mario Deep Maker 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB19D63-5EFB-4455-AE55-3AF1C45F5E8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AF31AB-45C7-423A-9E8E-481D2F9D65A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20895" yWindow="4800" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="3525" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -4962,8 +4962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{173310C4-1295-4648-B14B-887801CC320C}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9352,10 +9352,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F57D332-C942-4E13-9976-905346472273}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9379,7 +9380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9393,7 +9394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9407,7 +9408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9421,7 +9422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9435,7 +9436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9449,7 +9450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -9463,7 +9464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9477,7 +9478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9491,7 +9492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9505,7 +9506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9519,7 +9520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9533,7 +9534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -9547,7 +9548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -9561,7 +9562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -9575,7 +9576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -9589,7 +9590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -9603,7 +9604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -9617,7 +9618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -9631,7 +9632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -9645,7 +9646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -9659,7 +9660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -9673,7 +9674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9687,7 +9688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9701,7 +9702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9715,7 +9716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9729,7 +9730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -9743,7 +9744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -9757,7 +9758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9771,7 +9772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -9785,7 +9786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -9799,7 +9800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -9813,7 +9814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -9827,7 +9828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -9841,7 +9842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -9855,7 +9856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -9869,7 +9870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -9883,7 +9884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -9897,7 +9898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -9911,7 +9912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -9925,7 +9926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -9939,7 +9940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -9953,7 +9954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -9967,7 +9968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -9981,7 +9982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -9995,7 +9996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -10009,7 +10010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -10023,7 +10024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -10037,7 +10038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -10051,7 +10052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -10065,7 +10066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -10079,7 +10080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -10093,7 +10094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -10107,7 +10108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -10121,7 +10122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -10135,7 +10136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -10149,7 +10150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -10163,7 +10164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -10177,7 +10178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -10191,7 +10192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -10205,7 +10206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -10219,7 +10220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -10233,7 +10234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -10247,7 +10248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -10261,7 +10262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -10275,7 +10276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -10289,7 +10290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -10303,7 +10304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -10317,7 +10318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -10331,7 +10332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -10345,7 +10346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -10359,7 +10360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -10373,7 +10374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -10387,7 +10388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -10401,7 +10402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -10415,7 +10416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -10429,7 +10430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -10443,7 +10444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -10457,7 +10458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -10471,7 +10472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -10485,7 +10486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -10499,7 +10500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -10513,7 +10514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -10527,7 +10528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -10555,7 +10556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -10569,7 +10570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -10583,7 +10584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -10597,7 +10598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -10611,7 +10612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -10625,7 +10626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -10639,7 +10640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -10653,7 +10654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -10667,7 +10668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -10681,7 +10682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -10695,7 +10696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -10709,7 +10710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -10723,7 +10724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -10737,7 +10738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -10751,7 +10752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -10765,7 +10766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -10779,7 +10780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -10793,7 +10794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -10807,7 +10808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -10821,7 +10822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -10835,7 +10836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -10849,7 +10850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -10863,7 +10864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -10877,7 +10878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -10891,7 +10892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -10905,7 +10906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -10919,7 +10920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -10933,7 +10934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -10947,7 +10948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -10961,7 +10962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -10975,7 +10976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -10989,7 +10990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -11003,7 +11004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -11017,7 +11018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -11031,7 +11032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -11045,7 +11046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -11059,7 +11060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -11073,7 +11074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -11087,7 +11088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -11101,7 +11102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -11115,7 +11116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -11129,7 +11130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -11158,7 +11159,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D128" xr:uid="{81A1C1DD-1FDE-48B4-9B47-D008B9EC1248}"/>
+  <autoFilter ref="A1:D128" xr:uid="{81A1C1DD-1FDE-48B4-9B47-D008B9EC1248}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Snake Block"/>
+        <filter val="snakeTrack"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Altri fix, superati i 300
</commit_message>
<xml_diff>
--- a/Analisi approfondita sovrapponibili.xlsx
+++ b/Analisi approfondita sovrapponibili.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documenti\repositories\Super Mario Deep Maker 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6EAB5E-325D-4EFD-B6BC-70F460791BD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8054CF-F98D-474D-8B26-B52B3B151CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="3525" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="3525" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -1040,8 +1040,8 @@
   <dimension ref="A1:T129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4962,8 +4962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{173310C4-1295-4648-B14B-887801CC320C}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5172,8 +5172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E01B41-BDA6-4A71-AD93-F66AD7291B52}">
   <dimension ref="A1:C128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C128"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Boo su nuvola da risolvere, 500 superati
</commit_message>
<xml_diff>
--- a/Analisi approfondita sovrapponibili.xlsx
+++ b/Analisi approfondita sovrapponibili.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documenti\repositories\Super Mario Deep Maker 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8054CF-F98D-474D-8B26-B52B3B151CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E397EAE-B739-43BC-AE4F-7E12A8CB8E9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4830" yWindow="3525" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="165">
   <si>
     <t>Nome</t>
   </si>
@@ -532,6 +532,12 @@
   </si>
   <si>
     <t>snakeTrack</t>
+  </si>
+  <si>
+    <t>soundEffects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oggetti in tubo </t>
   </si>
 </sst>
 </file>
@@ -4960,10 +4966,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{173310C4-1295-4648-B14B-887801CC320C}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5161,6 +5167,22 @@
       </c>
       <c r="B26">
         <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>